<commit_message>
practice properties file read and write
</commit_message>
<xml_diff>
--- a/AbhishekClasses/src/main/resources/students.xlsx
+++ b/AbhishekClasses/src/main/resources/students.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="45">
   <si>
     <t>Student Id</t>
   </si>
@@ -162,6 +162,15 @@
   </si>
   <si>
     <t>sabina@gmail.com</t>
+  </si>
+  <si>
+    <t>dfa</t>
+  </si>
+  <si>
+    <t>fasd</t>
+  </si>
+  <si>
+    <t>34</t>
   </si>
 </sst>
 </file>
@@ -544,7 +553,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D43FDD0F-223E-4C50-945D-A71D5F5B43A7}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H1" sqref="H1:K23"/>
@@ -880,6 +889,38 @@
         <v>41</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="n" s="0">
+        <v>101.0</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="C11" t="n" s="0">
+        <v>33.0</v>
+      </c>
+      <c r="D11" t="n" s="0">
+        <v>32.0</v>
+      </c>
+      <c r="E11" t="n" s="0">
+        <v>32.0</v>
+      </c>
+      <c r="F11" t="n" s="0">
+        <v>44.0</v>
+      </c>
+      <c r="G11" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="H11" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="I11" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="J11" t="s" s="0">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>